<commit_message>
GUI SKETCH V3 upload
</commit_message>
<xml_diff>
--- a/관리산출물/관리산출물PMP PSP/PMP_개발진척관리.xlsx
+++ b/관리산출물/관리산출물PMP PSP/PMP_개발진척관리.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGTSeo\Documents\GitHub\sinsudong-crusher-home\관리산출물\관리산출물PMP PSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813CF4FA-4BC1-4FFA-8BE6-181588013C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E70263E-64AA-402F-9B12-6D16F266E4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2350" windowWidth="19030" windowHeight="14440" activeTab="1" xr2:uid="{35ECD954-CA6E-4E6A-B3FF-BD8FAAD43E44}"/>
+    <workbookView xWindow="7790" yWindow="980" windowWidth="19030" windowHeight="14440" activeTab="2" xr2:uid="{35ECD954-CA6E-4E6A-B3FF-BD8FAAD43E44}"/>
   </bookViews>
   <sheets>
     <sheet name="관리산출물" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>SRS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,19 +147,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>지역 입력기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>통신기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>클라우드 업로드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정보 통신기능</t>
+    <t>로그인 성공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아요버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>싫어요 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로고침버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설문조사 화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역추천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피드백 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피드백 후 새로고침 반영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Json을 사용한 데이터 Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Json을 이용한 데이터 Output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -579,10 +619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42F8919-F5F3-4342-BDC3-8497FF0FCE6C}">
-  <dimension ref="B3:F45"/>
+  <dimension ref="B3:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -590,6 +630,7 @@
     <col min="3" max="3" width="18.75" customWidth="1"/>
     <col min="4" max="4" width="30.9140625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.45">
@@ -623,125 +664,207 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>25</v>
       </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>18</v>
       </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>19</v>
       </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>20</v>
       </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>21</v>
       </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>22</v>
       </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>23</v>
       </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>24</v>
       </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C24" t="s">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C25" t="s">
+      <c r="E33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C26" t="s">
+      <c r="E37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C27" t="s">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C33" t="s">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D34" t="s">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D35" t="s">
+      <c r="E43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D45" t="s">
-        <v>30</v>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -749,7 +872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093AC475-F174-4525-8C3E-8F19472F0D31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData/>
@@ -768,12 +893,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101009E3EDE6BE485F24E9212E4628E3D8D2C" ma:contentTypeVersion="6" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="ca23bc866d5a207a3baad68403270f03">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dbddbc75-87a7-4d67-b143-ac604e4a65cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85b4551e07356f6e33910c22b2ee8e8f" ns3:_="">
     <xsd:import namespace="dbddbc75-87a7-4d67-b143-ac604e4a65cf"/>
@@ -931,6 +1050,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB066DA-1415-4CF0-9F70-7F8FEBB1910D}">
   <ds:schemaRefs>
@@ -940,22 +1065,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2A5E52-0DD3-4F99-B228-5D1C7062C1B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="dbddbc75-87a7-4d67-b143-ac604e4a65cf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F74DF39C-094C-40C0-9829-21CB5058FD67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -971,4 +1080,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2A5E52-0DD3-4F99-B228-5D1C7062C1B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="dbddbc75-87a7-4d67-b143-ac604e4a65cf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>